<commit_message>
Update Functionality Tests Results.xlsx
New test results
</commit_message>
<xml_diff>
--- a/Functionality Tests Results.xlsx
+++ b/Functionality Tests Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\AppData\Local\GitHubDesktop\app-2.9.6\Mechanical_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF1A2B1-5B45-4A50-BE35-C329D518F6D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787AA07E-DDD8-4633-978C-DDA9C7AB63F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1144,7 +1144,7 @@
         <v>686.7</v>
       </c>
       <c r="D2" s="25">
-        <f t="shared" ref="D2:D34" si="0">B2-C2</f>
+        <f t="shared" ref="D2:D24" si="0">B2-C2</f>
         <v>0</v>
       </c>
       <c r="E2" s="24" t="s">
@@ -1157,7 +1157,7 @@
         <v>686.7</v>
       </c>
       <c r="H2" s="25">
-        <f>F2-G2</f>
+        <f t="shared" ref="H2:H11" si="1">F2-G2</f>
         <v>0</v>
       </c>
     </row>
@@ -1185,7 +1185,7 @@
         <v>686.7</v>
       </c>
       <c r="H3" s="25">
-        <f>F3-G3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1213,7 +1213,7 @@
         <v>686.7</v>
       </c>
       <c r="H4" s="25">
-        <f>F4-G4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1241,7 +1241,7 @@
         <v>686.7</v>
       </c>
       <c r="H5" s="25">
-        <f>F5-G5</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1269,7 +1269,7 @@
         <v>686.7</v>
       </c>
       <c r="H6" s="25">
-        <f>F6-G6</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1297,7 +1297,7 @@
         <v>686.7</v>
       </c>
       <c r="H7" s="25">
-        <f>F7-G7</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1325,7 +1325,7 @@
         <v>686.7</v>
       </c>
       <c r="H8" s="25">
-        <f>F8-G8</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1353,7 +1353,7 @@
         <v>686.7</v>
       </c>
       <c r="H9" s="25">
-        <f>F9-G9</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1381,7 +1381,7 @@
         <v>686.7</v>
       </c>
       <c r="H10" s="25">
-        <f>F10-G10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1409,7 +1409,7 @@
         <v>686.7</v>
       </c>
       <c r="H11" s="28">
-        <f>F11-G11</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1619,7 +1619,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>